<commit_message>
Added a draft in word, some figures, etc.
Changed to word so I could do some fine-tune edits.
</commit_message>
<xml_diff>
--- a/paper/documentation and planning/master to-do.xlsx
+++ b/paper/documentation and planning/master to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwal5\Documents\GitHub\SMAREACTcleaned\paper\documentation and planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274C0DBC-CF45-4343-A154-33B570B58328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C376B22-42E0-4A8E-9C7E-B478CE80B453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
   </bookViews>
@@ -24,12 +24,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>Notes</t>
   </si>
@@ -205,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add a table with the two calibration parameters. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got it drafted on paper. Move to inkscape now. Maybe play with the aspect ratios to get everything down. </t>
   </si>
 </sst>
 </file>
@@ -283,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -343,30 +356,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -396,302 +390,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFCE4D6"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1024,7 +722,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1120,7 +818,7 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1133,61 +831,75 @@
       <c r="E5" s="15">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F5" s="15">
+        <v>0.125</v>
+      </c>
+      <c r="G5" s="17">
+        <v>45426</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="15">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F6" s="3"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="3"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="10" t="s">
-        <v>34</v>
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="15">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -1197,7 +909,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="15">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F9" s="15">
         <v>1.0416666666666666E-2</v>
@@ -1207,9 +919,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
@@ -1229,34 +941,36 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="15">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="F11" s="15">
-        <v>1.0416666666666666E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
@@ -1266,88 +980,78 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F12" s="15">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G12" s="17">
+        <v>45235</v>
+      </c>
       <c r="H12" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="15">
-        <v>0.125</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F13" s="15">
-        <v>0.10416666666666667</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F14" s="15">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G14" s="17">
-        <v>45235</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="15">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F15" s="15">
-        <v>4.1666666666666664E-2</v>
-      </c>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
@@ -1359,47 +1063,59 @@
       <c r="E16" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="F16" s="15">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G16" s="17">
+        <v>45236</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="15">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G17" s="17">
+        <v>45405</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F18" s="15">
-        <v>3.125E-2</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="G18" s="17">
-        <v>45236</v>
+        <v>45405</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>40</v>
@@ -1556,7 +1272,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="9">
         <f>COUNT(F2:F25)/COUNT(E2:E25)</f>
-        <v>0.59090909090909094</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -1570,20 +1286,20 @@
       <c r="D27" s="6"/>
       <c r="E27" s="11">
         <f>SUM(E2:E25)</f>
-        <v>1.4583333333333333</v>
+        <v>1.458333333333333</v>
       </c>
       <c r="F27" s="11">
         <f>SUM(F2:F25)</f>
-        <v>0.61805555555555558</v>
+        <v>0.75694444444444442</v>
       </c>
       <c r="G27" s="6"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H24">
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="7"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="6"/>
     <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="5"/>
     <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="2"/>
     <sortCondition ref="C2:C24" customList="Intro,Methods,Example,Conclusion"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1644,8 +1360,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A3">
-    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="44"/>
-    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="43"/>
+    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Quality of life edits
Basic wordsmithing, not focused. Got to page 6/16
</commit_message>
<xml_diff>
--- a/paper/documentation and planning/master to-do.xlsx
+++ b/paper/documentation and planning/master to-do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwal5\Documents\GitHub\SMAREACTcleaned\paper\documentation and planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C376B22-42E0-4A8E-9C7E-B478CE80B453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D42EC7C-A550-42AB-8909-EC6560179A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="First Draft" sheetId="4" r:id="rId1"/>
@@ -722,7 +722,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Move draft to v3
</commit_message>
<xml_diff>
--- a/paper/documentation and planning/master to-do.xlsx
+++ b/paper/documentation and planning/master to-do.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwal5\Documents\GitHub\SMAREACTcleaned\paper\documentation and planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D42EC7C-A550-42AB-8909-EC6560179A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DAF917-C3E0-41A8-8D90-57EFD4459606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="First Draft" sheetId="4" r:id="rId1"/>
-    <sheet name="Citations to add" sheetId="7" r:id="rId2"/>
+    <sheet name="Second Draft" sheetId="8" r:id="rId2"/>
+    <sheet name="Citations to add" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'First Draft'!$A$1:$H$1</definedName>
@@ -24,22 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
   <si>
     <t>Notes</t>
   </si>
@@ -218,6 +209,153 @@
   </si>
   <si>
     <t xml:space="preserve">Got it drafted on paper. Move to inkscape now. Maybe play with the aspect ratios to get everything down. </t>
+  </si>
+  <si>
+    <t>Add a few sentences about why SMAs are used (high work energy density), specifically highlighting the actuator properties.</t>
+  </si>
+  <si>
+    <t>Clean up the "current tools" paragraph</t>
+  </si>
+  <si>
+    <t>Should we change "preprocessing" to "processing" to take a less model-centric perspective?</t>
+  </si>
+  <si>
+    <t>Talk to Jacob?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Figures/Org</t>
+  </si>
+  <si>
+    <t>Collect citations on optimization for SMA model calibration</t>
+  </si>
+  <si>
+    <t>Consider deleting first paragraph in model calibration</t>
+  </si>
+  <si>
+    <t>Pedro/Whitten/Walgren/Bertagne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just read through to make sure it flows. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd paragraph in model calibration: Move the last sentence to be the topic sentence. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure it flows and make sure I'm not saying the same thing twice. </t>
+  </si>
+  <si>
+    <t>Collect references on analytical calibration methods for SMAs</t>
+  </si>
+  <si>
+    <t>Model calibration, paragraph 5: Have I mentioned material property interdependence before now?</t>
+  </si>
+  <si>
+    <t>Think about organization with figure 2 (SMA-REACT description). Does this belong in its own section?</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a sentence or two about our intended audience for the paper (we write this paper for…). That allows us to scope the mathematical details of the paper. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">From that scoping, I'll know how much detail we'll need to provide on the Lagoudas constitutive model. </t>
+  </si>
+  <si>
+    <t>Methods -&gt; 1D Constitutive Model: Is this section a primer on SMAs constitutive models, or on how you need numerical optimization for calibration?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"alternatively, we can discuss…" - Topic sentence mismatch. Rewrite to match what is written below (where each parameter shows up in the plot). </t>
+  </si>
+  <si>
+    <t>Do I need to divide model parameters into free variables and specified quantities?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask Jacob to see if we can get a preprint of the SMA book chapter on calibration. </t>
+  </si>
+  <si>
+    <t>Do I need to combine the model description section with the sequential calibration section?</t>
+  </si>
+  <si>
+    <t>Get a citation for how to select the calibration stress</t>
+  </si>
+  <si>
+    <t>Get a citation for how in most cases the H_min and sigma_crit are zero.</t>
+  </si>
+  <si>
+    <t>Just look through the book or other examples. This makes sense, because you'll either get grain realignment or you won't…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The statement about how the ASTM standard defines properties in a different manner than the Lagoudas model is buried in a paragraph. Pull that out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe move this up to a section about why we need a separate calibration tool. </t>
+  </si>
+  <si>
+    <t>"In past work,…" move this to a more relevant section. Maybe to the introduction? Maybe cut it in general?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the entire model description section for any mathematical rationale that doesn't have the accompanying math. </t>
+  </si>
+  <si>
+    <t>In the SMA development process, do we need to introduce roles and personas for each person doing a different stage of the work?</t>
+  </si>
+  <si>
+    <t>Intro + Methods</t>
+  </si>
+  <si>
+    <t>If we introduce different personas and decide on titles, that'll make explaining the model calibration part much easier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change iterative calibration/conventional calibration to sequential? Because both are iterative. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure out something that Jacob can understand. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look through the ASTM standard to pull a quick discussion about what stress levels to pick out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep it succint. This isn't an SMA characterization paper. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Think about moving the sequential calibration procedure to the appendix or to combine it with the model description section. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">See what Jacob thinks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the conventional/sequential calibration figures better aspect ratios. </t>
+  </si>
+  <si>
+    <t>Figures</t>
+  </si>
+  <si>
+    <t>Add a branched function to the H_cur function</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just google it. </t>
+  </si>
+  <si>
+    <t>Add the data for the bounds on the concurrent/global calibration section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just look through the JSON files. </t>
+  </si>
+  <si>
+    <t>Pull Bigelow's figure for the non-constant stress influence coefficients. Also think about how this works, because the model should capture some of these changes (quadratic with stress)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe could just delete this part. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trim the model/calibration deficencies paragraph(s). The calibration is pretty damn good. </t>
   </si>
 </sst>
 </file>
@@ -296,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -355,6 +493,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFA5CE4-38C8-47E4-9265-D715D6A32031}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1308,6 +1452,647 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B460BD39-EF2D-4B69-BAAC-25E1DDA445B4}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="40.06640625" customWidth="1"/>
+    <col min="2" max="3" width="13.9296875" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.06640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="39.265625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F6" s="21">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="G6" s="22">
+        <v>45453</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.125</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="15">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="21">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="21">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="21">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="21">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="21">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="21">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="21">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A28" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="21">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A32" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="9">
+        <f>COUNT(F2:F34)/COUNT(E2:E34)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="11">
+        <f>SUM(E2:E34)</f>
+        <v>0.92013888888888906</v>
+      </c>
+      <c r="F36" s="11">
+        <f>SUM(F2:F6)</f>
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H33">
+    <sortCondition ref="C2:C33" customList="Intro,Intro + Methods,Methods,Example,Conclusion"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981837F4-49C3-4443-B8D3-C9F25727AA12}">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Reference updates and minor wordsmithing.
</commit_message>
<xml_diff>
--- a/paper/documentation and planning/master to-do.xlsx
+++ b/paper/documentation and planning/master to-do.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwal5\Documents\GitHub\SMAREACTcleaned\paper\documentation and planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DAF917-C3E0-41A8-8D90-57EFD4459606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435B7D18-5E00-4D22-B82B-8787F9FB1AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="103">
   <si>
     <t>Notes</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t xml:space="preserve">Trim the model/calibration deficencies paragraph(s). The calibration is pretty damn good. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emailed the contact at Abaqus, will probably add one more citation, but it's done. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The less we spend on this, the better. Everyone has heard about the SMA "magic material" way too much. </t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,71 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1440,10 +1510,10 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H24">
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="5"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="4"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="3"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="13"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="12"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="11"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="10"/>
     <sortCondition ref="C2:C24" customList="Intro,Methods,Example,Conclusion"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1456,7 +1526,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1496,30 +1566,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="15">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2"/>
+      <c r="E2" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -1527,37 +1597,37 @@
       <c r="D3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="15">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="21">
-        <v>4.1666666666666664E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -1570,90 +1640,89 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="18" t="s">
-        <v>58</v>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E6" s="21">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F6" s="21">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="G6" s="22">
-        <v>45453</v>
-      </c>
       <c r="H6" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="21">
-        <v>1.7361111111111112E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.125</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="21">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E8" s="15">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="E9" s="21">
-        <v>2.0833333333333332E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
@@ -1661,37 +1730,32 @@
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0.125</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D10" s="3"/>
+      <c r="E10" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="15">
-        <v>6.25E-2</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="3"/>
+      <c r="E11" s="21">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -1703,13 +1767,10 @@
       <c r="E12" s="21">
         <v>3.125E-2</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
@@ -1721,16 +1782,13 @@
       <c r="E13" s="21">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
@@ -1740,9 +1798,9 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
@@ -1752,122 +1810,125 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="21">
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E16" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="21">
-        <v>3.125E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="21">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="21">
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="21">
-        <v>1.0416666666666666E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="21">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
@@ -1875,17 +1936,19 @@
       <c r="C23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E23" s="21">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
@@ -1895,12 +1958,15 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="21">
-        <v>1.3888888888888888E-2</v>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
@@ -1908,52 +1974,52 @@
       <c r="C25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E25" s="21">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H25" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="21">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="10" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>9</v>
@@ -1961,22 +2027,20 @@
       <c r="C28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="21">
-        <v>3.125E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>24</v>
@@ -1985,78 +2049,101 @@
       <c r="E29" s="21">
         <v>1.7361111111111112E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H29" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="10" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="21">
+        <v>1.7361111111111112E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A31" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F31" s="15">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="21">
-        <v>1.7361111111111112E-2</v>
+      <c r="G31" s="17">
+        <v>45519</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="57" x14ac:dyDescent="0.45">
-      <c r="A32" s="10" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="21">
-        <v>1.7361111111111112E-2</v>
+      <c r="E32" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F32" s="15">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G32" s="17">
+        <v>45519</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A33" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="21">
-        <v>1.7361111111111112E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F33" s="21">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="G33" s="22">
+        <v>45453</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>6</v>
       </c>
@@ -2065,10 +2152,10 @@
       <c r="D35" s="6"/>
       <c r="E35" s="9">
         <f>COUNT(F2:F34)/COUNT(E2:E34)</f>
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -2077,16 +2164,17 @@
       <c r="D36" s="6"/>
       <c r="E36" s="11">
         <f>SUM(E2:E34)</f>
-        <v>0.92013888888888906</v>
+        <v>0.92013888888888895</v>
       </c>
       <c r="F36" s="11">
         <f>SUM(F2:F6)</f>
-        <v>6.9444444444444441E-3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H33">
-    <sortCondition ref="C2:C33" customList="Intro,Intro + Methods,Methods,Example,Conclusion"/>
+    <sortCondition sortBy="cellColor" ref="A2:A33" dxfId="3"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="A2:A33" dxfId="2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2145,8 +2233,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A3">
-    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="1"/>
-    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="0"/>
+    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="9"/>
+    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Another edit push. Cleaning up the to-do list.
</commit_message>
<xml_diff>
--- a/paper/documentation and planning/master to-do.xlsx
+++ b/paper/documentation and planning/master to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwal5\Documents\GitHub\SMAREACTcleaned\paper\documentation and planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8289A6DC-4668-4434-A95D-B553C5A430D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65758AE7-F071-42ED-85F2-4C244CCA5643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{4AA8D39A-3EBC-4E51-A267-B07E4FB98F1F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="106">
   <si>
     <t>Notes</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Intro + Methods</t>
   </si>
   <si>
-    <t>If we introduce different personas and decide on titles, that'll make explaining the model calibration part much easier.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Change iterative calibration/conventional calibration to sequential? Because both are iterative. </t>
   </si>
   <si>
@@ -325,9 +322,6 @@
     <t xml:space="preserve">Think about moving the sequential calibration procedure to the appendix or to combine it with the model description section. </t>
   </si>
   <si>
-    <t xml:space="preserve">See what Jacob thinks. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Make the conventional/sequential calibration figures better aspect ratios. </t>
   </si>
   <si>
@@ -362,6 +356,21 @@
   </si>
   <si>
     <t xml:space="preserve">The less we spend on this, the better. Everyone has heard about the SMA "magic material" way too much. </t>
+  </si>
+  <si>
+    <t>It's a short paragraph.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See what Jacob thinks. I like it there. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think it flows incredibly now. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleted it. Unncessary. </t>
+  </si>
+  <si>
+    <t>If we introduce different personas and decide on titles, that'll make explaining the model calibration part much easier. Nope.</t>
   </si>
 </sst>
 </file>
@@ -510,11 +519,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
+          <fgColor rgb="FFE2EFDA"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -531,6 +540,38 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1462,10 +1503,10 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H24">
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="7"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="6"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="5"/>
-    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="11"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="10"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="9"/>
+    <sortCondition sortBy="cellColor" ref="A2:A24" dxfId="8"/>
     <sortCondition ref="C2:C24" customList="Intro,Methods,Example,Conclusion"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1477,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B460BD39-EF2D-4B69-BAAC-25E1DDA445B4}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1597,7 +1638,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="18" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1612,8 +1653,14 @@
       <c r="E6" s="21">
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="F6" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G6" s="22">
+        <v>45533</v>
+      </c>
       <c r="H6" s="12" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1735,9 +1782,9 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
@@ -1747,62 +1794,65 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="21">
-        <v>3.125E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E15" s="21">
-        <v>2.0833333333333332E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="21">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="21">
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>24</v>
@@ -1811,28 +1861,28 @@
       <c r="E18" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
+      <c r="H18" s="12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="21">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
@@ -1842,15 +1892,12 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="21">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>79</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
@@ -1858,14 +1905,19 @@
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E21" s="21">
-        <v>1.3888888888888888E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
@@ -1875,32 +1927,30 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="21">
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>86</v>
+        <v>1.7361111111111112E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="10" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
@@ -1910,15 +1960,15 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="21">
-        <v>2.0833333333333332E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
-        <v>89</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A25" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
@@ -1926,70 +1976,97 @@
       <c r="C25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="21">
         <v>3.125E-2</v>
       </c>
+      <c r="F25" s="21">
+        <v>0</v>
+      </c>
+      <c r="G25" s="22">
+        <v>45533</v>
+      </c>
       <c r="H25" s="12" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
-        <v>91</v>
+      <c r="A26" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="21">
-        <v>1.7361111111111112E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
-        <v>93</v>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F26" s="21">
+        <v>0</v>
+      </c>
+      <c r="G26" s="22">
+        <v>45533</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A27" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E27" s="21">
-        <v>1.0416666666666666E-2</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F27" s="21">
+        <v>0</v>
+      </c>
+      <c r="G27" s="22">
+        <v>45533</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="10" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="18" t="s">
+        <v>91</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="21">
-        <v>1.7361111111111112E-2</v>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F28" s="21">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="G28" s="22">
+        <v>45533</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="57" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
-        <v>98</v>
+      <c r="A29" s="18" t="s">
+        <v>96</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>9</v>
@@ -2001,13 +2078,19 @@
       <c r="E29" s="21">
         <v>1.7361111111111112E-2</v>
       </c>
+      <c r="F29" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G29" s="22">
+        <v>45533</v>
+      </c>
       <c r="H29" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A30" s="10" t="s">
-        <v>100</v>
+      <c r="A30" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>9</v>
@@ -2019,6 +2102,15 @@
       <c r="E30" s="21">
         <v>1.7361111111111112E-2</v>
       </c>
+      <c r="F30" s="21">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="G30" s="22">
+        <v>45533</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="18" t="s">
@@ -2043,7 +2135,7 @@
         <v>45519</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -2067,7 +2159,7 @@
         <v>45519</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -2104,7 +2196,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="9">
         <f>COUNT(F2:F34)/COUNT(E2:E34)</f>
-        <v>9.375E-2</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -2120,7 +2212,7 @@
       </c>
       <c r="F36" s="11">
         <f>SUM(F2:F6)</f>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2185,8 +2277,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A3">
-    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="1"/>
-    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="0"/>
+    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="7"/>
+    <sortCondition sortBy="cellColor" ref="A2:A3" dxfId="6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>